<commit_message>
Modifing the PP and RTM documents according to the new deliveries of HSI & CYRS: - Mapping the new CYRS & HSI to the CRS in the RTM - Updating the PP with the new progress Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BAAF5F-54DB-4B31-B365-1E54735F25F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE837C-66F8-4EF6-BC5B-7F4590DC7D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -593,38 +593,38 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:AP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,61 +1091,61 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="J2" s="27">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="J2" s="29">
         <v>43831</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29">
         <v>43862</v>
       </c>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
       <c r="J3" s="8">
         <v>21</v>
       </c>
@@ -1378,25 +1378,25 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="27" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="7" t="s">
@@ -1440,25 +1440,25 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="27" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="7" t="s">
@@ -1502,25 +1502,25 @@
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="27" t="s">
         <v>37</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -1564,25 +1564,25 @@
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="27" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="7" t="s">
@@ -1626,25 +1626,25 @@
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="27" t="s">
         <v>37</v>
       </c>
       <c r="I9" s="7" t="s">
@@ -1688,25 +1688,25 @@
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="27" t="s">
         <v>37</v>
       </c>
       <c r="I10" s="7" t="s">
@@ -1750,25 +1750,25 @@
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="27" t="s">
         <v>52</v>
       </c>
       <c r="I11" s="7" t="s">
@@ -1812,25 +1812,25 @@
       <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="27" t="s">
         <v>52</v>
       </c>
       <c r="I12" s="7" t="s">
@@ -1874,25 +1874,25 @@
       <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="27" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="7" t="s">
@@ -1936,25 +1936,25 @@
       <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="27" t="s">
         <v>46</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -1998,25 +1998,25 @@
       <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="36"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="7" t="s">
         <v>38</v>
       </c>
@@ -2033,9 +2033,9 @@
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
+      <c r="W15" s="22"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
       <c r="Z15" s="14"/>
       <c r="AA15" s="14"/>
       <c r="AB15" s="14"/>
@@ -2058,25 +2058,25 @@
       <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="36"/>
+      <c r="H16" s="27"/>
       <c r="I16" s="7" t="s">
         <v>38</v>
       </c>
@@ -2095,8 +2095,8 @@
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
       <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
       <c r="AC16" s="14"/>
@@ -2118,25 +2118,25 @@
       <c r="A17" s="6">
         <v>13</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="36"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="7" t="s">
         <v>38</v>
       </c>
@@ -2155,8 +2155,8 @@
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
       <c r="AC17" s="14"/>
@@ -2178,25 +2178,25 @@
       <c r="A18" s="6">
         <v>14</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="36"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="7" t="s">
         <v>38</v>
       </c>
@@ -2213,9 +2213,9 @@
       <c r="T18" s="14"/>
       <c r="U18" s="14"/>
       <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="14"/>
       <c r="AB18" s="14"/>
@@ -2238,25 +2238,25 @@
       <c r="A19" s="6">
         <v>15</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="36"/>
+      <c r="H19" s="27"/>
       <c r="I19" s="7" t="s">
         <v>38</v>
       </c>
@@ -2273,9 +2273,9 @@
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="14"/>
       <c r="AB19" s="14"/>
@@ -2296,30 +2296,30 @@
     </row>
     <row r="20" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J20" s="20"/>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J21" s="19"/>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J22" s="25"/>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2388,26 +2388,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="35"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>

</xml_diff>

<commit_message>
Updating the PP with new tasks after the delivery of the SRS document Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE837C-66F8-4EF6-BC5B-7F4590DC7D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368A6988-8553-4077-8D42-F7A9CCC3D67C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>7-2-2020</t>
+  </si>
+  <si>
+    <t>6-2-2020</t>
+  </si>
+  <si>
+    <t>7-3-2020</t>
+  </si>
+  <si>
+    <t>Modifing the CYRS Document acoording to our last team review meeting (6-2-2020)</t>
+  </si>
+  <si>
+    <t>Modifing the SRS Document acoording to our last team review meeting (6-2-2020)</t>
+  </si>
+  <si>
+    <t>Modifing the HSI Document acoording to our last team review meeting (6-2-2020)</t>
+  </si>
+  <si>
+    <t>Modifing the HSI Document acoording to our last  team review meeting (6-2-2020)</t>
   </si>
 </sst>
 </file>
@@ -515,45 +533,12 @@
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,62 +554,95 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,1272 +1079,1582 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:AP22"/>
+  <dimension ref="A1:AP27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15:V15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="21" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="29" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="43" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="50" style="19" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="21" width="3" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="2" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="2" style="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="43" width="3" style="19" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="36" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="J2" s="29">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="J2" s="20">
         <v>43831</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20">
         <v>43862</v>
       </c>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
-      <c r="AG2" s="29"/>
-      <c r="AH2" s="29"/>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="29"/>
-      <c r="AP2" s="29"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="J3" s="8">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="J3" s="21">
         <v>21</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="22">
         <v>22</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="22">
         <v>23</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="22">
         <v>24</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="22">
         <v>25</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="22">
         <v>26</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="22">
         <v>27</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="Q3" s="22">
         <v>28</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="22">
         <v>29</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="22">
         <v>30</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="22">
         <v>31</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="22">
         <v>1</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="22">
         <v>2</v>
       </c>
-      <c r="W3" s="9">
+      <c r="W3" s="22">
         <v>3</v>
       </c>
-      <c r="X3" s="9">
+      <c r="X3" s="22">
         <v>4</v>
       </c>
-      <c r="Y3" s="9">
+      <c r="Y3" s="22">
         <v>5</v>
       </c>
-      <c r="Z3" s="9">
+      <c r="Z3" s="22">
         <v>6</v>
       </c>
-      <c r="AA3" s="9">
+      <c r="AA3" s="22">
         <v>7</v>
       </c>
-      <c r="AB3" s="9">
+      <c r="AB3" s="22">
         <v>8</v>
       </c>
-      <c r="AC3" s="9">
+      <c r="AC3" s="22">
         <v>9</v>
       </c>
-      <c r="AD3" s="9">
+      <c r="AD3" s="22">
         <v>10</v>
       </c>
-      <c r="AE3" s="9">
+      <c r="AE3" s="22">
         <v>11</v>
       </c>
-      <c r="AF3" s="9">
+      <c r="AF3" s="22">
         <v>12</v>
       </c>
-      <c r="AG3" s="9">
+      <c r="AG3" s="22">
         <v>13</v>
       </c>
-      <c r="AH3" s="9">
+      <c r="AH3" s="22">
         <v>14</v>
       </c>
-      <c r="AI3" s="9">
+      <c r="AI3" s="22">
         <v>15</v>
       </c>
-      <c r="AJ3" s="9">
+      <c r="AJ3" s="22">
         <v>16</v>
       </c>
-      <c r="AK3" s="9">
+      <c r="AK3" s="22">
         <v>17</v>
       </c>
-      <c r="AL3" s="9">
+      <c r="AL3" s="22">
         <v>18</v>
       </c>
-      <c r="AM3" s="9">
+      <c r="AM3" s="22">
         <v>19</v>
       </c>
-      <c r="AN3" s="9">
+      <c r="AN3" s="22">
         <v>20</v>
       </c>
-      <c r="AO3" s="9">
+      <c r="AO3" s="22">
         <v>21</v>
       </c>
-      <c r="AP3" s="10">
+      <c r="AP3" s="23">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="12" t="s">
+      <c r="U4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="V4" s="12" t="s">
+      <c r="V4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="X4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="12" t="s">
+      <c r="Y4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="Z4" s="12" t="s">
+      <c r="Z4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="12" t="s">
+      <c r="AB4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="12" t="s">
+      <c r="AC4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AD4" s="12" t="s">
+      <c r="AD4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AE4" s="12" t="s">
+      <c r="AE4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AF4" s="12" t="s">
+      <c r="AF4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AG4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AH4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="12" t="s">
+      <c r="AI4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AJ4" s="12" t="s">
+      <c r="AJ4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="AK4" s="12" t="s">
+      <c r="AK4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="12" t="s">
+      <c r="AL4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AM4" s="12" t="s">
+      <c r="AM4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="AN4" s="12" t="s">
+      <c r="AN4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AO4" s="12" t="s">
+      <c r="AO4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AP4" s="13" t="s">
+      <c r="AP4" s="27" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="14"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
     </row>
     <row r="6" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="28">
         <v>2</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+      <c r="AN6" s="29"/>
+      <c r="AO6" s="29"/>
+      <c r="AP6" s="29"/>
     </row>
     <row r="7" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="28">
         <v>3</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
-      <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="14"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="14"/>
-      <c r="AM7" s="14"/>
-      <c r="AN7" s="14"/>
-      <c r="AO7" s="14"/>
-      <c r="AP7" s="14"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="29"/>
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
     </row>
     <row r="8" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
-      <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
-      <c r="AI8" s="14"/>
-      <c r="AJ8" s="14"/>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="14"/>
-      <c r="AN8" s="14"/>
-      <c r="AO8" s="14"/>
-      <c r="AP8" s="14"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="29"/>
+      <c r="AM8" s="29"/>
+      <c r="AN8" s="29"/>
+      <c r="AO8" s="29"/>
+      <c r="AP8" s="29"/>
     </row>
     <row r="9" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="28">
         <v>5</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
-      <c r="AH9" s="14"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
-      <c r="AO9" s="14"/>
-      <c r="AP9" s="14"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="29"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="29"/>
+      <c r="AN9" s="29"/>
+      <c r="AO9" s="29"/>
+      <c r="AP9" s="29"/>
     </row>
     <row r="10" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="28">
         <v>6</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
-      <c r="AG10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AO10" s="14"/>
-      <c r="AP10" s="14"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="29"/>
+      <c r="AN10" s="29"/>
+      <c r="AO10" s="29"/>
+      <c r="AP10" s="29"/>
     </row>
     <row r="11" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="28">
         <v>7</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
-      <c r="AO11" s="14"/>
-      <c r="AP11" s="14"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="29"/>
+      <c r="AE11" s="29"/>
+      <c r="AF11" s="29"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="29"/>
+      <c r="AI11" s="29"/>
+      <c r="AJ11" s="29"/>
+      <c r="AK11" s="29"/>
+      <c r="AL11" s="29"/>
+      <c r="AM11" s="29"/>
+      <c r="AN11" s="29"/>
+      <c r="AO11" s="29"/>
+      <c r="AP11" s="29"/>
     </row>
     <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="28">
         <v>8</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
-      <c r="AG12" s="14"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="14"/>
-      <c r="AJ12" s="14"/>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="14"/>
-      <c r="AP12" s="14"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="29"/>
+      <c r="AN12" s="29"/>
+      <c r="AO12" s="29"/>
+      <c r="AP12" s="29"/>
     </row>
     <row r="13" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="28">
         <v>9</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
-      <c r="AG13" s="14"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="14"/>
-      <c r="AJ13" s="14"/>
-      <c r="AK13" s="14"/>
-      <c r="AL13" s="14"/>
-      <c r="AM13" s="14"/>
-      <c r="AN13" s="14"/>
-      <c r="AO13" s="14"/>
-      <c r="AP13" s="14"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
+      <c r="AE13" s="29"/>
+      <c r="AF13" s="29"/>
+      <c r="AG13" s="29"/>
+      <c r="AH13" s="29"/>
+      <c r="AI13" s="29"/>
+      <c r="AJ13" s="29"/>
+      <c r="AK13" s="29"/>
+      <c r="AL13" s="29"/>
+      <c r="AM13" s="29"/>
+      <c r="AN13" s="29"/>
+      <c r="AO13" s="29"/>
+      <c r="AP13" s="29"/>
     </row>
     <row r="14" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="28">
         <v>10</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="14"/>
-      <c r="AG14" s="14"/>
-      <c r="AH14" s="14"/>
-      <c r="AI14" s="14"/>
-      <c r="AJ14" s="14"/>
-      <c r="AK14" s="14"/>
-      <c r="AL14" s="14"/>
-      <c r="AM14" s="14"/>
-      <c r="AN14" s="14"/>
-      <c r="AO14" s="14"/>
-      <c r="AP14" s="14"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29"/>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="29"/>
+      <c r="AN14" s="29"/>
+      <c r="AO14" s="29"/>
+      <c r="AP14" s="29"/>
     </row>
     <row r="15" spans="1:42" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="28">
         <v>11</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="7" t="s">
+      <c r="H15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
-      <c r="AG15" s="14"/>
-      <c r="AH15" s="14"/>
-      <c r="AI15" s="14"/>
-      <c r="AJ15" s="14"/>
-      <c r="AK15" s="14"/>
-      <c r="AL15" s="14"/>
-      <c r="AM15" s="14"/>
-      <c r="AN15" s="14"/>
-      <c r="AO15" s="14"/>
-      <c r="AP15" s="14"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="29"/>
+      <c r="AD15" s="29"/>
+      <c r="AE15" s="29"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="29"/>
+      <c r="AN15" s="29"/>
+      <c r="AO15" s="29"/>
+      <c r="AP15" s="29"/>
     </row>
     <row r="16" spans="1:42" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="28">
         <v>12</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="14"/>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="14"/>
-      <c r="AI16" s="14"/>
-      <c r="AJ16" s="14"/>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="14"/>
-      <c r="AM16" s="14"/>
-      <c r="AN16" s="14"/>
-      <c r="AO16" s="14"/>
-      <c r="AP16" s="14"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="29"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="29"/>
+      <c r="AN16" s="29"/>
+      <c r="AO16" s="29"/>
+      <c r="AP16" s="29"/>
     </row>
     <row r="17" spans="1:42" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="28">
         <v>13</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="7" t="s">
+      <c r="H17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
-      <c r="AG17" s="14"/>
-      <c r="AH17" s="14"/>
-      <c r="AI17" s="14"/>
-      <c r="AJ17" s="14"/>
-      <c r="AK17" s="14"/>
-      <c r="AL17" s="14"/>
-      <c r="AM17" s="14"/>
-      <c r="AN17" s="14"/>
-      <c r="AO17" s="14"/>
-      <c r="AP17" s="14"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="29"/>
+      <c r="AN17" s="29"/>
+      <c r="AO17" s="29"/>
+      <c r="AP17" s="29"/>
     </row>
     <row r="18" spans="1:42" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="28">
         <v>14</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="7" t="s">
+      <c r="H18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
-      <c r="AG18" s="14"/>
-      <c r="AH18" s="14"/>
-      <c r="AI18" s="14"/>
-      <c r="AJ18" s="14"/>
-      <c r="AK18" s="14"/>
-      <c r="AL18" s="14"/>
-      <c r="AM18" s="14"/>
-      <c r="AN18" s="14"/>
-      <c r="AO18" s="14"/>
-      <c r="AP18" s="14"/>
-    </row>
-    <row r="19" spans="1:42" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+      <c r="AC18" s="29"/>
+      <c r="AD18" s="29"/>
+      <c r="AE18" s="29"/>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="29"/>
+      <c r="AI18" s="29"/>
+      <c r="AJ18" s="29"/>
+      <c r="AK18" s="29"/>
+      <c r="AL18" s="29"/>
+      <c r="AM18" s="29"/>
+      <c r="AN18" s="29"/>
+      <c r="AO18" s="29"/>
+      <c r="AP18" s="29"/>
+    </row>
+    <row r="19" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
         <v>15</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="7" t="s">
+      <c r="H19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
-      <c r="AG19" s="14"/>
-      <c r="AH19" s="14"/>
-      <c r="AI19" s="14"/>
-      <c r="AJ19" s="14"/>
-      <c r="AK19" s="14"/>
-      <c r="AL19" s="14"/>
-      <c r="AM19" s="14"/>
-      <c r="AN19" s="14"/>
-      <c r="AO19" s="14"/>
-      <c r="AP19" s="14"/>
-    </row>
-    <row r="20" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="20"/>
-      <c r="K20" s="30" t="s">
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="29"/>
+      <c r="AF19" s="29"/>
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="29"/>
+      <c r="AI19" s="29"/>
+      <c r="AJ19" s="29"/>
+      <c r="AK19" s="29"/>
+      <c r="AL19" s="29"/>
+      <c r="AM19" s="29"/>
+      <c r="AN19" s="29"/>
+      <c r="AO19" s="29"/>
+      <c r="AP19" s="29"/>
+    </row>
+    <row r="20" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="28">
+        <v>16</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="30"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="29"/>
+      <c r="AI20" s="29"/>
+      <c r="AJ20" s="29"/>
+      <c r="AK20" s="29"/>
+      <c r="AL20" s="29"/>
+      <c r="AM20" s="29"/>
+      <c r="AN20" s="29"/>
+      <c r="AO20" s="29"/>
+      <c r="AP20" s="29"/>
+    </row>
+    <row r="21" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
+        <v>17</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29"/>
+      <c r="AI21" s="29"/>
+      <c r="AJ21" s="29"/>
+      <c r="AK21" s="29"/>
+      <c r="AL21" s="29"/>
+      <c r="AM21" s="29"/>
+      <c r="AN21" s="29"/>
+      <c r="AO21" s="29"/>
+      <c r="AP21" s="29"/>
+    </row>
+    <row r="22" spans="1:42" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="28">
+        <v>18</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="29"/>
+      <c r="AN22" s="29"/>
+      <c r="AO22" s="29"/>
+      <c r="AP22" s="29"/>
+    </row>
+    <row r="23" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="28">
+        <v>19</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="29"/>
+      <c r="AB23" s="29"/>
+      <c r="AC23" s="29"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="29"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="29"/>
+      <c r="AI23" s="29"/>
+      <c r="AJ23" s="29"/>
+      <c r="AK23" s="29"/>
+      <c r="AL23" s="29"/>
+      <c r="AM23" s="29"/>
+      <c r="AN23" s="29"/>
+      <c r="AO23" s="29"/>
+      <c r="AP23" s="29"/>
+    </row>
+    <row r="24" spans="1:42" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28">
+        <v>20</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="30"/>
+      <c r="AA24" s="29"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+      <c r="AM24" s="29"/>
+      <c r="AN24" s="29"/>
+      <c r="AO24" s="29"/>
+      <c r="AP24" s="29"/>
+    </row>
+    <row r="25" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="35"/>
+      <c r="K25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-    </row>
-    <row r="21" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="19"/>
-      <c r="K21" s="32" t="s">
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+    </row>
+    <row r="26" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="36"/>
+      <c r="K26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-    </row>
-    <row r="22" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" s="25"/>
-      <c r="K22" s="34" t="s">
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="37"/>
+      <c r="K27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
     <mergeCell ref="U2:AP2"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K25:N25"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="J2:T2"/>
   </mergeCells>
@@ -2386,200 +2714,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="37" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updating the pp by assigning new tasks to the SRS document. Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300DBEF3-31EA-4192-8C8E-3E58EF12B530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3835B7C-3F04-4A64-805F-2179B657CF69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
   <si>
     <t>#</t>
   </si>
@@ -251,6 +251,15 @@
   </si>
   <si>
     <t>Modifing the HSI Document acoording to our last  team review meeting (6-2-2020)</t>
+  </si>
+  <si>
+    <t>Modifing the SRS Document by adding the context diagram</t>
+  </si>
+  <si>
+    <t>17-2-2020</t>
+  </si>
+  <si>
+    <t>20-2-2020</t>
   </si>
 </sst>
 </file>
@@ -531,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -614,6 +623,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -641,7 +653,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1079,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:AP27"/>
+  <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H24"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,18 +1117,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="35" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -1155,57 +1167,57 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="32">
+      <c r="J2" s="33">
         <v>43831</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33">
         <v>43862</v>
       </c>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11">
@@ -2614,7 +2626,7 @@
       <c r="AO23" s="19"/>
       <c r="AP23" s="19"/>
     </row>
-    <row r="24" spans="1:42" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2676,39 +2688,297 @@
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
     </row>
-    <row r="25" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J25" s="25"/>
-      <c r="K25" s="33" t="s">
+    <row r="25" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>21</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+      <c r="AG25" s="19"/>
+      <c r="AH25" s="19"/>
+      <c r="AI25" s="19"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="20"/>
+      <c r="AL25" s="19"/>
+      <c r="AM25" s="19"/>
+      <c r="AN25" s="19"/>
+      <c r="AO25" s="19"/>
+      <c r="AP25" s="19"/>
+    </row>
+    <row r="26" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>22</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+      <c r="AG26" s="19"/>
+      <c r="AH26" s="19"/>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="19"/>
+      <c r="AM26" s="19"/>
+      <c r="AN26" s="19"/>
+      <c r="AO26" s="19"/>
+      <c r="AP26" s="19"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>23</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="19"/>
+      <c r="AP27" s="19"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>24</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="19"/>
+      <c r="AP28" s="19"/>
+    </row>
+    <row r="29" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>25</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="19"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
+      <c r="AL29" s="19"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="19"/>
+      <c r="AP29" s="19"/>
+    </row>
+    <row r="30" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="25"/>
+      <c r="K30" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-    </row>
-    <row r="26" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J26" s="26"/>
-      <c r="K26" s="28" t="s">
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+    </row>
+    <row r="31" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="26"/>
+      <c r="K31" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-    </row>
-    <row r="27" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="27"/>
-      <c r="K27" s="30" t="s">
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="27"/>
+      <c r="K32" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
     <mergeCell ref="U2:AP2"/>
-    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K30:N30"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="J2:T2"/>
   </mergeCells>
@@ -2770,26 +3040,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="36"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updating the PP by assing tasks to edit and review the SRS Also updating the RTM after last commits Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3835B7C-3F04-4A64-805F-2179B657CF69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE562623-4595-481F-96B1-25588C930E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="86">
   <si>
     <t>#</t>
   </si>
@@ -103,9 +103,6 @@
     <t>SRS_v1.0</t>
   </si>
   <si>
-    <t>HIS_v1.0</t>
-  </si>
-  <si>
     <t>RTM_v1.0</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>SRS_v1.1</t>
   </si>
   <si>
-    <t>HIS_v1.1</t>
-  </si>
-  <si>
     <t>31-1-2020</t>
   </si>
   <si>
@@ -260,6 +254,42 @@
   </si>
   <si>
     <t>20-2-2020</t>
+  </si>
+  <si>
+    <t>Partially done</t>
+  </si>
+  <si>
+    <t>21-2-2020</t>
+  </si>
+  <si>
+    <t>22-2-2020</t>
+  </si>
+  <si>
+    <t>Modifing the SRS Document by modifing the context diagram</t>
+  </si>
+  <si>
+    <t>Modifing the SRS Document by updating the requirements according to the reviewer comments</t>
+  </si>
+  <si>
+    <t>SRS-Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewing the SRS document </t>
+  </si>
+  <si>
+    <t>23-2-2020</t>
+  </si>
+  <si>
+    <t>CYRS_v1.4</t>
+  </si>
+  <si>
+    <t>HSI_v1.1</t>
+  </si>
+  <si>
+    <t>HSI_v1.0</t>
+  </si>
+  <si>
+    <t>HSI_v1.5</t>
   </si>
 </sst>
 </file>
@@ -540,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,6 +656,9 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,7 +686,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,7 +780,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1028701</xdr:colOff>
+      <xdr:colOff>971551</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -1093,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:AP32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI24" sqref="AI24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1140,7 @@
     <col min="6" max="6" width="17.140625" style="10" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="21" width="3" style="10" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="2" style="10" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -1121,11 +1154,11 @@
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -1167,57 +1200,57 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="33">
+      <c r="J2" s="34">
         <v>43831</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33">
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34">
         <v>43862</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11">
@@ -1331,7 +1364,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>3</v>
@@ -1453,28 +1486,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="I5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="20"/>
@@ -1515,16 +1548,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>20</v>
@@ -1533,10 +1566,10 @@
         <v>20</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
@@ -1577,28 +1610,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="G7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
@@ -1639,28 +1672,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="I8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="20"/>
@@ -1701,28 +1734,28 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
@@ -1763,28 +1796,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -1825,28 +1858,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="H11" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -1887,28 +1920,28 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="H12" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -1949,28 +1982,28 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="I13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -2011,28 +2044,28 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="I14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -2073,28 +2106,28 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="H15" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -2135,28 +2168,28 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="I16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -2197,28 +2230,28 @@
         <v>13</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="I17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -2259,28 +2292,28 @@
         <v>14</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="H18" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -2321,28 +2354,28 @@
         <v>15</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="I19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -2383,28 +2416,28 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
@@ -2445,28 +2478,28 @@
         <v>17</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -2507,28 +2540,28 @@
         <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
@@ -2569,28 +2602,28 @@
         <v>19</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
@@ -2631,28 +2664,28 @@
         <v>20</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
@@ -2693,26 +2726,28 @@
         <v>21</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="H25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
@@ -2742,9 +2777,9 @@
       <c r="AI25" s="19"/>
       <c r="AJ25" s="19"/>
       <c r="AK25" s="20"/>
-      <c r="AL25" s="19"/>
-      <c r="AM25" s="19"/>
-      <c r="AN25" s="19"/>
+      <c r="AL25" s="20"/>
+      <c r="AM25" s="20"/>
+      <c r="AN25" s="20"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
     </row>
@@ -2753,26 +2788,28 @@
         <v>22</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="H26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
@@ -2802,24 +2839,38 @@
       <c r="AI26" s="19"/>
       <c r="AJ26" s="19"/>
       <c r="AK26" s="20"/>
-      <c r="AL26" s="19"/>
-      <c r="AM26" s="19"/>
-      <c r="AN26" s="19"/>
+      <c r="AL26" s="20"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
       <c r="AO26" s="19"/>
       <c r="AP26" s="19"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>23</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
+      <c r="B27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29" t="s">
+        <v>37</v>
+      </c>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
@@ -2851,21 +2902,35 @@
       <c r="AL27" s="19"/>
       <c r="AM27" s="19"/>
       <c r="AN27" s="19"/>
-      <c r="AO27" s="19"/>
+      <c r="AO27" s="20"/>
       <c r="AP27" s="19"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>24</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
+      <c r="B28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29" t="s">
+        <v>37</v>
+      </c>
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
@@ -2897,21 +2962,33 @@
       <c r="AL28" s="19"/>
       <c r="AM28" s="19"/>
       <c r="AN28" s="19"/>
-      <c r="AO28" s="19"/>
+      <c r="AO28" s="20"/>
       <c r="AP28" s="19"/>
     </row>
-    <row r="29" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>25</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
+      <c r="B29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
@@ -2948,30 +3025,30 @@
     </row>
     <row r="30" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J30" s="25"/>
-      <c r="K30" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
+      <c r="K30" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J31" s="26"/>
-      <c r="K31" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
+      <c r="K31" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
     </row>
     <row r="32" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J32" s="27"/>
-      <c r="K32" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
+      <c r="K32" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3021,15 +3098,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84E9320-5BEB-4411-BFD0-20ED4C434367}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
@@ -3040,26 +3117,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
@@ -3100,7 +3177,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,7 +3197,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3128,7 +3205,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
@@ -3140,7 +3217,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3148,7 +3225,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
@@ -3160,7 +3237,7 @@
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3168,19 +3245,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3188,19 +3265,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3208,30 +3285,100 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updating both the PP and the RTM according to the new deliveries Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE562623-4595-481F-96B1-25588C930E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5645DB3-F5BF-4792-AA9F-8114D4DC8DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="96">
   <si>
     <t>#</t>
   </si>
@@ -290,6 +290,36 @@
   </si>
   <si>
     <t>HSI_v1.5</t>
+  </si>
+  <si>
+    <t>26-2-2020</t>
+  </si>
+  <si>
+    <t>25-2-2020</t>
+  </si>
+  <si>
+    <t>Context diagram needs modifications and test scope needs removing</t>
+  </si>
+  <si>
+    <t>Initiating the GDD document</t>
+  </si>
+  <si>
+    <t>Creating the static architecture section in the GDD</t>
+  </si>
+  <si>
+    <t>Creating the APIs section in the GDD</t>
+  </si>
+  <si>
+    <t>24-2-2020</t>
+  </si>
+  <si>
+    <t>26-3-2020</t>
+  </si>
+  <si>
+    <t>27-3-2020</t>
+  </si>
+  <si>
+    <t>Modifing the SRS Document by removing test scopes section</t>
   </si>
 </sst>
 </file>
@@ -366,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,6 +695,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -686,7 +725,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1124,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:AP32"/>
+  <dimension ref="A1:BL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,27 +1177,27 @@
     <col min="4" max="4" width="50" style="10" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="10" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="10" customWidth="1"/>
     <col min="10" max="21" width="3" style="10" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="2" style="10" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="25" max="29" width="2" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="43" width="3" style="10" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="10"/>
+    <col min="30" max="49" width="3" style="10" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -1195,62 +1234,86 @@
       <c r="AO1" s="19"/>
       <c r="AP1" s="19"/>
     </row>
-    <row r="2" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="34">
+      <c r="J2" s="35">
         <v>43831</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34">
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35">
         <v>43862</v>
       </c>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-    </row>
-    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="35"/>
+      <c r="AP2" s="35"/>
+      <c r="AQ2" s="35">
+        <v>43891</v>
+      </c>
+      <c r="AR2" s="35"/>
+      <c r="AS2" s="35"/>
+      <c r="AT2" s="35"/>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
+      <c r="AY2" s="35"/>
+      <c r="AZ2" s="35"/>
+      <c r="BA2" s="35"/>
+      <c r="BB2" s="35"/>
+      <c r="BC2" s="35"/>
+      <c r="BD2" s="35"/>
+      <c r="BE2" s="35"/>
+      <c r="BF2" s="35"/>
+      <c r="BG2" s="35"/>
+      <c r="BH2" s="35"/>
+      <c r="BI2" s="35"/>
+      <c r="BJ2" s="35"/>
+      <c r="BK2" s="35"/>
+      <c r="BL2" s="35"/>
+    </row>
+    <row r="3" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11">
@@ -1352,8 +1415,29 @@
       <c r="AP3" s="13">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="12">
+        <v>23</v>
+      </c>
+      <c r="AR3" s="13">
+        <v>24</v>
+      </c>
+      <c r="AS3" s="12">
+        <v>25</v>
+      </c>
+      <c r="AT3" s="13">
+        <v>26</v>
+      </c>
+      <c r="AU3" s="13">
+        <v>27</v>
+      </c>
+      <c r="AV3" s="12">
+        <v>28</v>
+      </c>
+      <c r="AW3" s="13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
@@ -1480,8 +1564,29 @@
       <c r="AP4" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW4" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>1</v>
       </c>
@@ -1542,8 +1647,15 @@
       <c r="AN5" s="19"/>
       <c r="AO5" s="19"/>
       <c r="AP5" s="19"/>
-    </row>
-    <row r="6" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="19"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+    </row>
+    <row r="6" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>2</v>
       </c>
@@ -1604,8 +1716,15 @@
       <c r="AN6" s="19"/>
       <c r="AO6" s="19"/>
       <c r="AP6" s="19"/>
-    </row>
-    <row r="7" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AT6" s="19"/>
+      <c r="AU6" s="19"/>
+      <c r="AV6" s="19"/>
+      <c r="AW6" s="19"/>
+    </row>
+    <row r="7" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>3</v>
       </c>
@@ -1666,8 +1785,15 @@
       <c r="AN7" s="19"/>
       <c r="AO7" s="19"/>
       <c r="AP7" s="19"/>
-    </row>
-    <row r="8" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="19"/>
+      <c r="AS7" s="19"/>
+      <c r="AT7" s="19"/>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="19"/>
+      <c r="AW7" s="19"/>
+    </row>
+    <row r="8" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>4</v>
       </c>
@@ -1728,8 +1854,15 @@
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
       <c r="AP8" s="19"/>
-    </row>
-    <row r="9" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AQ8" s="19"/>
+      <c r="AR8" s="19"/>
+      <c r="AS8" s="19"/>
+      <c r="AT8" s="19"/>
+      <c r="AU8" s="19"/>
+      <c r="AV8" s="19"/>
+      <c r="AW8" s="19"/>
+    </row>
+    <row r="9" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>5</v>
       </c>
@@ -1790,8 +1923,15 @@
       <c r="AN9" s="19"/>
       <c r="AO9" s="19"/>
       <c r="AP9" s="19"/>
-    </row>
-    <row r="10" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="19"/>
+      <c r="AS9" s="19"/>
+      <c r="AT9" s="19"/>
+      <c r="AU9" s="19"/>
+      <c r="AV9" s="19"/>
+      <c r="AW9" s="19"/>
+    </row>
+    <row r="10" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>6</v>
       </c>
@@ -1852,8 +1992,15 @@
       <c r="AN10" s="19"/>
       <c r="AO10" s="19"/>
       <c r="AP10" s="19"/>
-    </row>
-    <row r="11" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ10" s="19"/>
+      <c r="AR10" s="19"/>
+      <c r="AS10" s="19"/>
+      <c r="AT10" s="19"/>
+      <c r="AU10" s="19"/>
+      <c r="AV10" s="19"/>
+      <c r="AW10" s="19"/>
+    </row>
+    <row r="11" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>7</v>
       </c>
@@ -1914,8 +2061,15 @@
       <c r="AN11" s="19"/>
       <c r="AO11" s="19"/>
       <c r="AP11" s="19"/>
-    </row>
-    <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ11" s="19"/>
+      <c r="AR11" s="19"/>
+      <c r="AS11" s="19"/>
+      <c r="AT11" s="19"/>
+      <c r="AU11" s="19"/>
+      <c r="AV11" s="19"/>
+      <c r="AW11" s="19"/>
+    </row>
+    <row r="12" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>8</v>
       </c>
@@ -1976,8 +2130,15 @@
       <c r="AN12" s="19"/>
       <c r="AO12" s="19"/>
       <c r="AP12" s="19"/>
-    </row>
-    <row r="13" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ12" s="19"/>
+      <c r="AR12" s="19"/>
+      <c r="AS12" s="19"/>
+      <c r="AT12" s="19"/>
+      <c r="AU12" s="19"/>
+      <c r="AV12" s="19"/>
+      <c r="AW12" s="19"/>
+    </row>
+    <row r="13" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>9</v>
       </c>
@@ -2038,8 +2199,15 @@
       <c r="AN13" s="19"/>
       <c r="AO13" s="19"/>
       <c r="AP13" s="19"/>
-    </row>
-    <row r="14" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="19"/>
+      <c r="AR13" s="19"/>
+      <c r="AS13" s="19"/>
+      <c r="AT13" s="19"/>
+      <c r="AU13" s="19"/>
+      <c r="AV13" s="19"/>
+      <c r="AW13" s="19"/>
+    </row>
+    <row r="14" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>10</v>
       </c>
@@ -2100,8 +2268,15 @@
       <c r="AN14" s="19"/>
       <c r="AO14" s="19"/>
       <c r="AP14" s="19"/>
-    </row>
-    <row r="15" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="AQ14" s="19"/>
+      <c r="AR14" s="19"/>
+      <c r="AS14" s="19"/>
+      <c r="AT14" s="19"/>
+      <c r="AU14" s="19"/>
+      <c r="AV14" s="19"/>
+      <c r="AW14" s="19"/>
+    </row>
+    <row r="15" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>11</v>
       </c>
@@ -2162,8 +2337,15 @@
       <c r="AN15" s="19"/>
       <c r="AO15" s="19"/>
       <c r="AP15" s="19"/>
-    </row>
-    <row r="16" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="AQ15" s="19"/>
+      <c r="AR15" s="19"/>
+      <c r="AS15" s="19"/>
+      <c r="AT15" s="19"/>
+      <c r="AU15" s="19"/>
+      <c r="AV15" s="19"/>
+      <c r="AW15" s="19"/>
+    </row>
+    <row r="16" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>12</v>
       </c>
@@ -2224,8 +2406,15 @@
       <c r="AN16" s="19"/>
       <c r="AO16" s="19"/>
       <c r="AP16" s="19"/>
-    </row>
-    <row r="17" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="AQ16" s="19"/>
+      <c r="AR16" s="19"/>
+      <c r="AS16" s="19"/>
+      <c r="AT16" s="19"/>
+      <c r="AU16" s="19"/>
+      <c r="AV16" s="19"/>
+      <c r="AW16" s="19"/>
+    </row>
+    <row r="17" spans="1:49" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>13</v>
       </c>
@@ -2286,8 +2475,15 @@
       <c r="AN17" s="19"/>
       <c r="AO17" s="19"/>
       <c r="AP17" s="19"/>
-    </row>
-    <row r="18" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="AQ17" s="19"/>
+      <c r="AR17" s="19"/>
+      <c r="AS17" s="19"/>
+      <c r="AT17" s="19"/>
+      <c r="AU17" s="19"/>
+      <c r="AV17" s="19"/>
+      <c r="AW17" s="19"/>
+    </row>
+    <row r="18" spans="1:49" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>14</v>
       </c>
@@ -2348,8 +2544,15 @@
       <c r="AN18" s="19"/>
       <c r="AO18" s="19"/>
       <c r="AP18" s="19"/>
-    </row>
-    <row r="19" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="AQ18" s="19"/>
+      <c r="AR18" s="19"/>
+      <c r="AS18" s="19"/>
+      <c r="AT18" s="19"/>
+      <c r="AU18" s="19"/>
+      <c r="AV18" s="19"/>
+      <c r="AW18" s="19"/>
+    </row>
+    <row r="19" spans="1:49" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>15</v>
       </c>
@@ -2410,8 +2613,15 @@
       <c r="AN19" s="19"/>
       <c r="AO19" s="19"/>
       <c r="AP19" s="19"/>
-    </row>
-    <row r="20" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ19" s="19"/>
+      <c r="AR19" s="19"/>
+      <c r="AS19" s="19"/>
+      <c r="AT19" s="19"/>
+      <c r="AU19" s="19"/>
+      <c r="AV19" s="19"/>
+      <c r="AW19" s="19"/>
+    </row>
+    <row r="20" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>16</v>
       </c>
@@ -2472,8 +2682,15 @@
       <c r="AN20" s="19"/>
       <c r="AO20" s="19"/>
       <c r="AP20" s="19"/>
-    </row>
-    <row r="21" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ20" s="19"/>
+      <c r="AR20" s="19"/>
+      <c r="AS20" s="19"/>
+      <c r="AT20" s="19"/>
+      <c r="AU20" s="19"/>
+      <c r="AV20" s="19"/>
+      <c r="AW20" s="19"/>
+    </row>
+    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>17</v>
       </c>
@@ -2534,8 +2751,15 @@
       <c r="AN21" s="19"/>
       <c r="AO21" s="19"/>
       <c r="AP21" s="19"/>
-    </row>
-    <row r="22" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ21" s="19"/>
+      <c r="AR21" s="19"/>
+      <c r="AS21" s="19"/>
+      <c r="AT21" s="19"/>
+      <c r="AU21" s="19"/>
+      <c r="AV21" s="19"/>
+      <c r="AW21" s="19"/>
+    </row>
+    <row r="22" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2596,8 +2820,15 @@
       <c r="AN22" s="19"/>
       <c r="AO22" s="19"/>
       <c r="AP22" s="19"/>
-    </row>
-    <row r="23" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ22" s="19"/>
+      <c r="AR22" s="19"/>
+      <c r="AS22" s="19"/>
+      <c r="AT22" s="19"/>
+      <c r="AU22" s="19"/>
+      <c r="AV22" s="19"/>
+      <c r="AW22" s="19"/>
+    </row>
+    <row r="23" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2658,8 +2889,15 @@
       <c r="AN23" s="19"/>
       <c r="AO23" s="19"/>
       <c r="AP23" s="19"/>
-    </row>
-    <row r="24" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="19"/>
+      <c r="AR23" s="19"/>
+      <c r="AS23" s="19"/>
+      <c r="AT23" s="19"/>
+      <c r="AU23" s="19"/>
+      <c r="AV23" s="19"/>
+      <c r="AW23" s="19"/>
+    </row>
+    <row r="24" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2720,8 +2958,15 @@
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
       <c r="AP24" s="19"/>
-    </row>
-    <row r="25" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ24" s="19"/>
+      <c r="AR24" s="19"/>
+      <c r="AS24" s="19"/>
+      <c r="AT24" s="19"/>
+      <c r="AU24" s="19"/>
+      <c r="AV24" s="19"/>
+      <c r="AW24" s="19"/>
+    </row>
+    <row r="25" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -2782,8 +3027,15 @@
       <c r="AN25" s="20"/>
       <c r="AO25" s="19"/>
       <c r="AP25" s="19"/>
-    </row>
-    <row r="26" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="19"/>
+      <c r="AS25" s="19"/>
+      <c r="AT25" s="19"/>
+      <c r="AU25" s="19"/>
+      <c r="AV25" s="19"/>
+      <c r="AW25" s="19"/>
+    </row>
+    <row r="26" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>22</v>
       </c>
@@ -2844,8 +3096,15 @@
       <c r="AN26" s="20"/>
       <c r="AO26" s="19"/>
       <c r="AP26" s="19"/>
-    </row>
-    <row r="27" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AQ26" s="19"/>
+      <c r="AR26" s="19"/>
+      <c r="AS26" s="19"/>
+      <c r="AT26" s="19"/>
+      <c r="AU26" s="19"/>
+      <c r="AV26" s="19"/>
+      <c r="AW26" s="19"/>
+    </row>
+    <row r="27" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>23</v>
       </c>
@@ -2867,7 +3126,9 @@
       <c r="G27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="I27" s="29" t="s">
         <v>37</v>
       </c>
@@ -2903,9 +3164,16 @@
       <c r="AM27" s="19"/>
       <c r="AN27" s="19"/>
       <c r="AO27" s="20"/>
-      <c r="AP27" s="19"/>
-    </row>
-    <row r="28" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+      <c r="AP27" s="20"/>
+      <c r="AQ27" s="21"/>
+      <c r="AR27" s="19"/>
+      <c r="AS27" s="19"/>
+      <c r="AT27" s="19"/>
+      <c r="AU27" s="19"/>
+      <c r="AV27" s="19"/>
+      <c r="AW27" s="19"/>
+    </row>
+    <row r="28" spans="1:49" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>24</v>
       </c>
@@ -2927,7 +3195,9 @@
       <c r="G28" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="29"/>
+      <c r="H28" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="I28" s="29" t="s">
         <v>37</v>
       </c>
@@ -2963,9 +3233,16 @@
       <c r="AM28" s="19"/>
       <c r="AN28" s="19"/>
       <c r="AO28" s="20"/>
-      <c r="AP28" s="19"/>
-    </row>
-    <row r="29" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="19"/>
+      <c r="AS28" s="19"/>
+      <c r="AT28" s="19"/>
+      <c r="AU28" s="19"/>
+      <c r="AV28" s="19"/>
+      <c r="AW28" s="19"/>
+    </row>
+    <row r="29" spans="1:49" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>25</v>
       </c>
@@ -2987,8 +3264,12 @@
       <c r="G29" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
+      <c r="H29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
@@ -3022,40 +3303,393 @@
       <c r="AN29" s="19"/>
       <c r="AO29" s="19"/>
       <c r="AP29" s="19"/>
-    </row>
-    <row r="30" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="25"/>
-      <c r="K30" s="35" t="s">
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="19"/>
+      <c r="AS29" s="19"/>
+      <c r="AT29" s="19"/>
+      <c r="AU29" s="19"/>
+      <c r="AV29" s="19"/>
+      <c r="AW29" s="19"/>
+    </row>
+    <row r="30" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
+        <v>26</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
+      <c r="AG30" s="19"/>
+      <c r="AH30" s="19"/>
+      <c r="AI30" s="19"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
+      <c r="AL30" s="19"/>
+      <c r="AM30" s="19"/>
+      <c r="AN30" s="19"/>
+      <c r="AO30" s="19"/>
+      <c r="AP30" s="19"/>
+      <c r="AQ30" s="19"/>
+      <c r="AR30" s="40"/>
+      <c r="AS30" s="40"/>
+      <c r="AT30" s="21"/>
+      <c r="AU30" s="19"/>
+      <c r="AV30" s="19"/>
+      <c r="AW30" s="19"/>
+    </row>
+    <row r="31" spans="1:49" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <v>27</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="19"/>
+      <c r="AI31" s="19"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
+      <c r="AL31" s="19"/>
+      <c r="AM31" s="19"/>
+      <c r="AN31" s="19"/>
+      <c r="AO31" s="19"/>
+      <c r="AP31" s="19"/>
+      <c r="AQ31" s="19"/>
+      <c r="AR31" s="40"/>
+      <c r="AS31" s="40"/>
+      <c r="AT31" s="19"/>
+      <c r="AU31" s="19"/>
+      <c r="AV31" s="19"/>
+      <c r="AW31" s="19"/>
+    </row>
+    <row r="32" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <v>28</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="19"/>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="19"/>
+      <c r="AI32" s="19"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
+      <c r="AL32" s="19"/>
+      <c r="AM32" s="19"/>
+      <c r="AN32" s="19"/>
+      <c r="AO32" s="19"/>
+      <c r="AP32" s="19"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="21"/>
+      <c r="AT32" s="19"/>
+      <c r="AU32" s="19"/>
+      <c r="AV32" s="19"/>
+      <c r="AW32" s="19"/>
+    </row>
+    <row r="33" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>29</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AF33" s="19"/>
+      <c r="AG33" s="19"/>
+      <c r="AH33" s="19"/>
+      <c r="AI33" s="19"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
+      <c r="AL33" s="19"/>
+      <c r="AM33" s="19"/>
+      <c r="AN33" s="19"/>
+      <c r="AO33" s="19"/>
+      <c r="AP33" s="19"/>
+      <c r="AQ33" s="19"/>
+      <c r="AR33" s="19"/>
+      <c r="AS33" s="20"/>
+      <c r="AT33" s="20"/>
+      <c r="AU33" s="19"/>
+      <c r="AV33" s="19"/>
+      <c r="AW33" s="19"/>
+    </row>
+    <row r="34" spans="1:49" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18">
+        <v>30</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="19"/>
+      <c r="AC34" s="19"/>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="19"/>
+      <c r="AF34" s="19"/>
+      <c r="AG34" s="19"/>
+      <c r="AH34" s="19"/>
+      <c r="AI34" s="19"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
+      <c r="AL34" s="19"/>
+      <c r="AM34" s="19"/>
+      <c r="AN34" s="19"/>
+      <c r="AO34" s="19"/>
+      <c r="AP34" s="19"/>
+      <c r="AQ34" s="19"/>
+      <c r="AR34" s="19"/>
+      <c r="AS34" s="20"/>
+      <c r="AT34" s="20"/>
+      <c r="AU34" s="21"/>
+      <c r="AV34" s="19"/>
+      <c r="AW34" s="19"/>
+    </row>
+    <row r="35" spans="1:49" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="25"/>
+      <c r="K35" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-    </row>
-    <row r="31" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J31" s="26"/>
-      <c r="K31" s="30" t="s">
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+    </row>
+    <row r="36" spans="1:49" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="26"/>
+      <c r="K36" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-    </row>
-    <row r="32" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J32" s="27"/>
-      <c r="K32" s="32" t="s">
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+    </row>
+    <row r="37" spans="1:49" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="27"/>
+      <c r="K37" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
+  <mergeCells count="7">
+    <mergeCell ref="AQ2:BL2"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K35:N35"/>
     <mergeCell ref="U2:AP2"/>
-    <mergeCell ref="K30:N30"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="J2:T2"/>
   </mergeCells>
@@ -3117,26 +3751,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="38"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
@@ -3307,16 +3941,16 @@
       <c r="B12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="30" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3327,16 +3961,16 @@
       <c r="B13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="30" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating the PP by assigning the tasks of creating LCD_CDD and DIO_SDD Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Elevator\Software Deliveries Log\PP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5645DB3-F5BF-4792-AA9F-8114D4DC8DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF328FA-B0FA-4D86-8828-7A85D360CB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="110">
   <si>
     <t>#</t>
   </si>
@@ -313,13 +313,55 @@
     <t>24-2-2020</t>
   </si>
   <si>
-    <t>26-3-2020</t>
-  </si>
-  <si>
-    <t>27-3-2020</t>
-  </si>
-  <si>
     <t>Modifing the SRS Document by removing test scopes section</t>
+  </si>
+  <si>
+    <t>GDD-Modifications</t>
+  </si>
+  <si>
+    <t>Updating the signals table and correcting the GDD documents header</t>
+  </si>
+  <si>
+    <t>28-2-2020</t>
+  </si>
+  <si>
+    <t>Updating the APIs section in the GDD</t>
+  </si>
+  <si>
+    <t>1-3-2020</t>
+  </si>
+  <si>
+    <t>29-2-2020</t>
+  </si>
+  <si>
+    <t>27-2-2020</t>
+  </si>
+  <si>
+    <t>Adding the inputs and outputs diagram</t>
+  </si>
+  <si>
+    <t>Completing the APIs section in the GDD</t>
+  </si>
+  <si>
+    <t>3-3-2020</t>
+  </si>
+  <si>
+    <t>4-3-2020</t>
+  </si>
+  <si>
+    <t>GDD-Creation</t>
+  </si>
+  <si>
+    <t>CDD-DIO-Creation</t>
+  </si>
+  <si>
+    <t>Initiating the CDD document for the DIO driver</t>
+  </si>
+  <si>
+    <t>Initiating the CDD document for the LCD driver</t>
+  </si>
+  <si>
+    <t>CDD-LCD-Creation</t>
   </si>
 </sst>
 </file>
@@ -698,6 +740,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,23 +761,14 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1163,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:BL37"/>
+  <dimension ref="A1:BL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1227,14 @@
     <col min="24" max="24" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="25" max="29" width="2" style="10" bestFit="1" customWidth="1"/>
     <col min="30" max="49" width="3" style="10" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="10"/>
+    <col min="50" max="50" width="2" style="10" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="2.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="2" style="10" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="3" style="10" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="2" style="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="2.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="59" max="64" width="3" style="10" bestFit="1" customWidth="1"/>
+    <col min="65" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,11 +1242,11 @@
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -1239,81 +1288,81 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="35">
+      <c r="J2" s="33">
         <v>43831</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33">
         <v>43862</v>
       </c>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
-      <c r="AL2" s="35"/>
-      <c r="AM2" s="35"/>
-      <c r="AN2" s="35"/>
-      <c r="AO2" s="35"/>
-      <c r="AP2" s="35"/>
-      <c r="AQ2" s="35">
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33">
         <v>43891</v>
       </c>
-      <c r="AR2" s="35"/>
-      <c r="AS2" s="35"/>
-      <c r="AT2" s="35"/>
-      <c r="AU2" s="35"/>
-      <c r="AV2" s="35"/>
-      <c r="AW2" s="35"/>
-      <c r="AX2" s="35"/>
-      <c r="AY2" s="35"/>
-      <c r="AZ2" s="35"/>
-      <c r="BA2" s="35"/>
-      <c r="BB2" s="35"/>
-      <c r="BC2" s="35"/>
-      <c r="BD2" s="35"/>
-      <c r="BE2" s="35"/>
-      <c r="BF2" s="35"/>
-      <c r="BG2" s="35"/>
-      <c r="BH2" s="35"/>
-      <c r="BI2" s="35"/>
-      <c r="BJ2" s="35"/>
-      <c r="BK2" s="35"/>
-      <c r="BL2" s="35"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="33"/>
+      <c r="AX2" s="33"/>
+      <c r="AY2" s="33"/>
+      <c r="AZ2" s="33"/>
+      <c r="BA2" s="33"/>
+      <c r="BB2" s="33"/>
+      <c r="BC2" s="33"/>
+      <c r="BD2" s="33"/>
+      <c r="BE2" s="33"/>
+      <c r="BF2" s="33"/>
+      <c r="BG2" s="33"/>
+      <c r="BH2" s="33"/>
+      <c r="BI2" s="33"/>
+      <c r="BJ2" s="33"/>
+      <c r="BK2" s="33"/>
+      <c r="BL2" s="33"/>
     </row>
     <row r="3" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11">
@@ -1436,6 +1485,51 @@
       <c r="AW3" s="13">
         <v>29</v>
       </c>
+      <c r="AX3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="13">
+        <v>2</v>
+      </c>
+      <c r="AZ3" s="13">
+        <v>3</v>
+      </c>
+      <c r="BA3" s="13">
+        <v>4</v>
+      </c>
+      <c r="BB3" s="13">
+        <v>5</v>
+      </c>
+      <c r="BC3" s="13">
+        <v>6</v>
+      </c>
+      <c r="BD3" s="13">
+        <v>7</v>
+      </c>
+      <c r="BE3" s="13">
+        <v>8</v>
+      </c>
+      <c r="BF3" s="13">
+        <v>9</v>
+      </c>
+      <c r="BG3" s="13">
+        <v>10</v>
+      </c>
+      <c r="BH3" s="13">
+        <v>11</v>
+      </c>
+      <c r="BI3" s="13">
+        <v>12</v>
+      </c>
+      <c r="BJ3" s="13">
+        <v>13</v>
+      </c>
+      <c r="BK3" s="13">
+        <v>14</v>
+      </c>
+      <c r="BL3" s="13">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -1584,6 +1678,51 @@
       </c>
       <c r="AW4" s="17" t="s">
         <v>11</v>
+      </c>
+      <c r="AX4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AZ4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="BC4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="BE4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="BG4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="BJ4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="BL4" s="16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
@@ -1654,6 +1793,20 @@
       <c r="AU5" s="19"/>
       <c r="AV5" s="19"/>
       <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+      <c r="AY5" s="19"/>
+      <c r="AZ5" s="19"/>
+      <c r="BA5" s="19"/>
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="19"/>
+      <c r="BF5" s="19"/>
+      <c r="BG5" s="19"/>
+      <c r="BH5" s="19"/>
+      <c r="BI5" s="19"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
     </row>
     <row r="6" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
@@ -1723,6 +1876,20 @@
       <c r="AU6" s="19"/>
       <c r="AV6" s="19"/>
       <c r="AW6" s="19"/>
+      <c r="AX6" s="19"/>
+      <c r="AY6" s="19"/>
+      <c r="AZ6" s="19"/>
+      <c r="BA6" s="19"/>
+      <c r="BB6" s="19"/>
+      <c r="BC6" s="19"/>
+      <c r="BD6" s="19"/>
+      <c r="BE6" s="19"/>
+      <c r="BF6" s="19"/>
+      <c r="BG6" s="19"/>
+      <c r="BH6" s="19"/>
+      <c r="BI6" s="19"/>
+      <c r="BJ6" s="19"/>
+      <c r="BK6" s="19"/>
     </row>
     <row r="7" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
@@ -1792,6 +1959,20 @@
       <c r="AU7" s="19"/>
       <c r="AV7" s="19"/>
       <c r="AW7" s="19"/>
+      <c r="AX7" s="19"/>
+      <c r="AY7" s="19"/>
+      <c r="AZ7" s="19"/>
+      <c r="BA7" s="19"/>
+      <c r="BB7" s="19"/>
+      <c r="BC7" s="19"/>
+      <c r="BD7" s="19"/>
+      <c r="BE7" s="19"/>
+      <c r="BF7" s="19"/>
+      <c r="BG7" s="19"/>
+      <c r="BH7" s="19"/>
+      <c r="BI7" s="19"/>
+      <c r="BJ7" s="19"/>
+      <c r="BK7" s="19"/>
     </row>
     <row r="8" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
@@ -1861,6 +2042,20 @@
       <c r="AU8" s="19"/>
       <c r="AV8" s="19"/>
       <c r="AW8" s="19"/>
+      <c r="AX8" s="19"/>
+      <c r="AY8" s="19"/>
+      <c r="AZ8" s="19"/>
+      <c r="BA8" s="19"/>
+      <c r="BB8" s="19"/>
+      <c r="BC8" s="19"/>
+      <c r="BD8" s="19"/>
+      <c r="BE8" s="19"/>
+      <c r="BF8" s="19"/>
+      <c r="BG8" s="19"/>
+      <c r="BH8" s="19"/>
+      <c r="BI8" s="19"/>
+      <c r="BJ8" s="19"/>
+      <c r="BK8" s="19"/>
     </row>
     <row r="9" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
@@ -1930,6 +2125,20 @@
       <c r="AU9" s="19"/>
       <c r="AV9" s="19"/>
       <c r="AW9" s="19"/>
+      <c r="AX9" s="19"/>
+      <c r="AY9" s="19"/>
+      <c r="AZ9" s="19"/>
+      <c r="BA9" s="19"/>
+      <c r="BB9" s="19"/>
+      <c r="BC9" s="19"/>
+      <c r="BD9" s="19"/>
+      <c r="BE9" s="19"/>
+      <c r="BF9" s="19"/>
+      <c r="BG9" s="19"/>
+      <c r="BH9" s="19"/>
+      <c r="BI9" s="19"/>
+      <c r="BJ9" s="19"/>
+      <c r="BK9" s="19"/>
     </row>
     <row r="10" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
@@ -1999,6 +2208,20 @@
       <c r="AU10" s="19"/>
       <c r="AV10" s="19"/>
       <c r="AW10" s="19"/>
+      <c r="AX10" s="19"/>
+      <c r="AY10" s="19"/>
+      <c r="AZ10" s="19"/>
+      <c r="BA10" s="19"/>
+      <c r="BB10" s="19"/>
+      <c r="BC10" s="19"/>
+      <c r="BD10" s="19"/>
+      <c r="BE10" s="19"/>
+      <c r="BF10" s="19"/>
+      <c r="BG10" s="19"/>
+      <c r="BH10" s="19"/>
+      <c r="BI10" s="19"/>
+      <c r="BJ10" s="19"/>
+      <c r="BK10" s="19"/>
     </row>
     <row r="11" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
@@ -2068,6 +2291,20 @@
       <c r="AU11" s="19"/>
       <c r="AV11" s="19"/>
       <c r="AW11" s="19"/>
+      <c r="AX11" s="19"/>
+      <c r="AY11" s="19"/>
+      <c r="AZ11" s="19"/>
+      <c r="BA11" s="19"/>
+      <c r="BB11" s="19"/>
+      <c r="BC11" s="19"/>
+      <c r="BD11" s="19"/>
+      <c r="BE11" s="19"/>
+      <c r="BF11" s="19"/>
+      <c r="BG11" s="19"/>
+      <c r="BH11" s="19"/>
+      <c r="BI11" s="19"/>
+      <c r="BJ11" s="19"/>
+      <c r="BK11" s="19"/>
     </row>
     <row r="12" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
@@ -2137,6 +2374,20 @@
       <c r="AU12" s="19"/>
       <c r="AV12" s="19"/>
       <c r="AW12" s="19"/>
+      <c r="AX12" s="19"/>
+      <c r="AY12" s="19"/>
+      <c r="AZ12" s="19"/>
+      <c r="BA12" s="19"/>
+      <c r="BB12" s="19"/>
+      <c r="BC12" s="19"/>
+      <c r="BD12" s="19"/>
+      <c r="BE12" s="19"/>
+      <c r="BF12" s="19"/>
+      <c r="BG12" s="19"/>
+      <c r="BH12" s="19"/>
+      <c r="BI12" s="19"/>
+      <c r="BJ12" s="19"/>
+      <c r="BK12" s="19"/>
     </row>
     <row r="13" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
@@ -2206,6 +2457,20 @@
       <c r="AU13" s="19"/>
       <c r="AV13" s="19"/>
       <c r="AW13" s="19"/>
+      <c r="AX13" s="19"/>
+      <c r="AY13" s="19"/>
+      <c r="AZ13" s="19"/>
+      <c r="BA13" s="19"/>
+      <c r="BB13" s="19"/>
+      <c r="BC13" s="19"/>
+      <c r="BD13" s="19"/>
+      <c r="BE13" s="19"/>
+      <c r="BF13" s="19"/>
+      <c r="BG13" s="19"/>
+      <c r="BH13" s="19"/>
+      <c r="BI13" s="19"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
     </row>
     <row r="14" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
@@ -2275,6 +2540,20 @@
       <c r="AU14" s="19"/>
       <c r="AV14" s="19"/>
       <c r="AW14" s="19"/>
+      <c r="AX14" s="19"/>
+      <c r="AY14" s="19"/>
+      <c r="AZ14" s="19"/>
+      <c r="BA14" s="19"/>
+      <c r="BB14" s="19"/>
+      <c r="BC14" s="19"/>
+      <c r="BD14" s="19"/>
+      <c r="BE14" s="19"/>
+      <c r="BF14" s="19"/>
+      <c r="BG14" s="19"/>
+      <c r="BH14" s="19"/>
+      <c r="BI14" s="19"/>
+      <c r="BJ14" s="19"/>
+      <c r="BK14" s="19"/>
     </row>
     <row r="15" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
@@ -2344,6 +2623,20 @@
       <c r="AU15" s="19"/>
       <c r="AV15" s="19"/>
       <c r="AW15" s="19"/>
+      <c r="AX15" s="19"/>
+      <c r="AY15" s="19"/>
+      <c r="AZ15" s="19"/>
+      <c r="BA15" s="19"/>
+      <c r="BB15" s="19"/>
+      <c r="BC15" s="19"/>
+      <c r="BD15" s="19"/>
+      <c r="BE15" s="19"/>
+      <c r="BF15" s="19"/>
+      <c r="BG15" s="19"/>
+      <c r="BH15" s="19"/>
+      <c r="BI15" s="19"/>
+      <c r="BJ15" s="19"/>
+      <c r="BK15" s="19"/>
     </row>
     <row r="16" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
@@ -2413,8 +2706,22 @@
       <c r="AU16" s="19"/>
       <c r="AV16" s="19"/>
       <c r="AW16" s="19"/>
-    </row>
-    <row r="17" spans="1:49" ht="45" x14ac:dyDescent="0.25">
+      <c r="AX16" s="19"/>
+      <c r="AY16" s="19"/>
+      <c r="AZ16" s="19"/>
+      <c r="BA16" s="19"/>
+      <c r="BB16" s="19"/>
+      <c r="BC16" s="19"/>
+      <c r="BD16" s="19"/>
+      <c r="BE16" s="19"/>
+      <c r="BF16" s="19"/>
+      <c r="BG16" s="19"/>
+      <c r="BH16" s="19"/>
+      <c r="BI16" s="19"/>
+      <c r="BJ16" s="19"/>
+      <c r="BK16" s="19"/>
+    </row>
+    <row r="17" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>13</v>
       </c>
@@ -2482,8 +2789,22 @@
       <c r="AU17" s="19"/>
       <c r="AV17" s="19"/>
       <c r="AW17" s="19"/>
-    </row>
-    <row r="18" spans="1:49" ht="45" x14ac:dyDescent="0.25">
+      <c r="AX17" s="19"/>
+      <c r="AY17" s="19"/>
+      <c r="AZ17" s="19"/>
+      <c r="BA17" s="19"/>
+      <c r="BB17" s="19"/>
+      <c r="BC17" s="19"/>
+      <c r="BD17" s="19"/>
+      <c r="BE17" s="19"/>
+      <c r="BF17" s="19"/>
+      <c r="BG17" s="19"/>
+      <c r="BH17" s="19"/>
+      <c r="BI17" s="19"/>
+      <c r="BJ17" s="19"/>
+      <c r="BK17" s="19"/>
+    </row>
+    <row r="18" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>14</v>
       </c>
@@ -2551,8 +2872,22 @@
       <c r="AU18" s="19"/>
       <c r="AV18" s="19"/>
       <c r="AW18" s="19"/>
-    </row>
-    <row r="19" spans="1:49" ht="45" x14ac:dyDescent="0.25">
+      <c r="AX18" s="19"/>
+      <c r="AY18" s="19"/>
+      <c r="AZ18" s="19"/>
+      <c r="BA18" s="19"/>
+      <c r="BB18" s="19"/>
+      <c r="BC18" s="19"/>
+      <c r="BD18" s="19"/>
+      <c r="BE18" s="19"/>
+      <c r="BF18" s="19"/>
+      <c r="BG18" s="19"/>
+      <c r="BH18" s="19"/>
+      <c r="BI18" s="19"/>
+      <c r="BJ18" s="19"/>
+      <c r="BK18" s="19"/>
+    </row>
+    <row r="19" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>15</v>
       </c>
@@ -2620,8 +2955,22 @@
       <c r="AU19" s="19"/>
       <c r="AV19" s="19"/>
       <c r="AW19" s="19"/>
-    </row>
-    <row r="20" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX19" s="19"/>
+      <c r="AY19" s="19"/>
+      <c r="AZ19" s="19"/>
+      <c r="BA19" s="19"/>
+      <c r="BB19" s="19"/>
+      <c r="BC19" s="19"/>
+      <c r="BD19" s="19"/>
+      <c r="BE19" s="19"/>
+      <c r="BF19" s="19"/>
+      <c r="BG19" s="19"/>
+      <c r="BH19" s="19"/>
+      <c r="BI19" s="19"/>
+      <c r="BJ19" s="19"/>
+      <c r="BK19" s="19"/>
+    </row>
+    <row r="20" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>16</v>
       </c>
@@ -2689,8 +3038,22 @@
       <c r="AU20" s="19"/>
       <c r="AV20" s="19"/>
       <c r="AW20" s="19"/>
-    </row>
-    <row r="21" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX20" s="19"/>
+      <c r="AY20" s="19"/>
+      <c r="AZ20" s="19"/>
+      <c r="BA20" s="19"/>
+      <c r="BB20" s="19"/>
+      <c r="BC20" s="19"/>
+      <c r="BD20" s="19"/>
+      <c r="BE20" s="19"/>
+      <c r="BF20" s="19"/>
+      <c r="BG20" s="19"/>
+      <c r="BH20" s="19"/>
+      <c r="BI20" s="19"/>
+      <c r="BJ20" s="19"/>
+      <c r="BK20" s="19"/>
+    </row>
+    <row r="21" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>17</v>
       </c>
@@ -2758,8 +3121,22 @@
       <c r="AU21" s="19"/>
       <c r="AV21" s="19"/>
       <c r="AW21" s="19"/>
-    </row>
-    <row r="22" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX21" s="19"/>
+      <c r="AY21" s="19"/>
+      <c r="AZ21" s="19"/>
+      <c r="BA21" s="19"/>
+      <c r="BB21" s="19"/>
+      <c r="BC21" s="19"/>
+      <c r="BD21" s="19"/>
+      <c r="BE21" s="19"/>
+      <c r="BF21" s="19"/>
+      <c r="BG21" s="19"/>
+      <c r="BH21" s="19"/>
+      <c r="BI21" s="19"/>
+      <c r="BJ21" s="19"/>
+      <c r="BK21" s="19"/>
+    </row>
+    <row r="22" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2827,8 +3204,22 @@
       <c r="AU22" s="19"/>
       <c r="AV22" s="19"/>
       <c r="AW22" s="19"/>
-    </row>
-    <row r="23" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX22" s="19"/>
+      <c r="AY22" s="19"/>
+      <c r="AZ22" s="19"/>
+      <c r="BA22" s="19"/>
+      <c r="BB22" s="19"/>
+      <c r="BC22" s="19"/>
+      <c r="BD22" s="19"/>
+      <c r="BE22" s="19"/>
+      <c r="BF22" s="19"/>
+      <c r="BG22" s="19"/>
+      <c r="BH22" s="19"/>
+      <c r="BI22" s="19"/>
+      <c r="BJ22" s="19"/>
+      <c r="BK22" s="19"/>
+    </row>
+    <row r="23" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2896,8 +3287,22 @@
       <c r="AU23" s="19"/>
       <c r="AV23" s="19"/>
       <c r="AW23" s="19"/>
-    </row>
-    <row r="24" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX23" s="19"/>
+      <c r="AY23" s="19"/>
+      <c r="AZ23" s="19"/>
+      <c r="BA23" s="19"/>
+      <c r="BB23" s="19"/>
+      <c r="BC23" s="19"/>
+      <c r="BD23" s="19"/>
+      <c r="BE23" s="19"/>
+      <c r="BF23" s="19"/>
+      <c r="BG23" s="19"/>
+      <c r="BH23" s="19"/>
+      <c r="BI23" s="19"/>
+      <c r="BJ23" s="19"/>
+      <c r="BK23" s="19"/>
+    </row>
+    <row r="24" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2965,8 +3370,22 @@
       <c r="AU24" s="19"/>
       <c r="AV24" s="19"/>
       <c r="AW24" s="19"/>
-    </row>
-    <row r="25" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX24" s="19"/>
+      <c r="AY24" s="19"/>
+      <c r="AZ24" s="19"/>
+      <c r="BA24" s="19"/>
+      <c r="BB24" s="19"/>
+      <c r="BC24" s="19"/>
+      <c r="BD24" s="19"/>
+      <c r="BE24" s="19"/>
+      <c r="BF24" s="19"/>
+      <c r="BG24" s="19"/>
+      <c r="BH24" s="19"/>
+      <c r="BI24" s="19"/>
+      <c r="BJ24" s="19"/>
+      <c r="BK24" s="19"/>
+    </row>
+    <row r="25" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -3034,8 +3453,22 @@
       <c r="AU25" s="19"/>
       <c r="AV25" s="19"/>
       <c r="AW25" s="19"/>
-    </row>
-    <row r="26" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX25" s="19"/>
+      <c r="AY25" s="19"/>
+      <c r="AZ25" s="19"/>
+      <c r="BA25" s="19"/>
+      <c r="BB25" s="19"/>
+      <c r="BC25" s="19"/>
+      <c r="BD25" s="19"/>
+      <c r="BE25" s="19"/>
+      <c r="BF25" s="19"/>
+      <c r="BG25" s="19"/>
+      <c r="BH25" s="19"/>
+      <c r="BI25" s="19"/>
+      <c r="BJ25" s="19"/>
+      <c r="BK25" s="19"/>
+    </row>
+    <row r="26" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>22</v>
       </c>
@@ -3103,8 +3536,22 @@
       <c r="AU26" s="19"/>
       <c r="AV26" s="19"/>
       <c r="AW26" s="19"/>
-    </row>
-    <row r="27" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX26" s="19"/>
+      <c r="AY26" s="19"/>
+      <c r="AZ26" s="19"/>
+      <c r="BA26" s="19"/>
+      <c r="BB26" s="19"/>
+      <c r="BC26" s="19"/>
+      <c r="BD26" s="19"/>
+      <c r="BE26" s="19"/>
+      <c r="BF26" s="19"/>
+      <c r="BG26" s="19"/>
+      <c r="BH26" s="19"/>
+      <c r="BI26" s="19"/>
+      <c r="BJ26" s="19"/>
+      <c r="BK26" s="19"/>
+    </row>
+    <row r="27" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>23</v>
       </c>
@@ -3172,8 +3619,22 @@
       <c r="AU27" s="19"/>
       <c r="AV27" s="19"/>
       <c r="AW27" s="19"/>
-    </row>
-    <row r="28" spans="1:49" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="AX27" s="19"/>
+      <c r="AY27" s="19"/>
+      <c r="AZ27" s="19"/>
+      <c r="BA27" s="19"/>
+      <c r="BB27" s="19"/>
+      <c r="BC27" s="19"/>
+      <c r="BD27" s="19"/>
+      <c r="BE27" s="19"/>
+      <c r="BF27" s="19"/>
+      <c r="BG27" s="19"/>
+      <c r="BH27" s="19"/>
+      <c r="BI27" s="19"/>
+      <c r="BJ27" s="19"/>
+      <c r="BK27" s="19"/>
+    </row>
+    <row r="28" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>24</v>
       </c>
@@ -3241,8 +3702,22 @@
       <c r="AU28" s="19"/>
       <c r="AV28" s="19"/>
       <c r="AW28" s="19"/>
-    </row>
-    <row r="29" spans="1:49" ht="60" x14ac:dyDescent="0.25">
+      <c r="AX28" s="19"/>
+      <c r="AY28" s="19"/>
+      <c r="AZ28" s="19"/>
+      <c r="BA28" s="19"/>
+      <c r="BB28" s="19"/>
+      <c r="BC28" s="19"/>
+      <c r="BD28" s="19"/>
+      <c r="BE28" s="19"/>
+      <c r="BF28" s="19"/>
+      <c r="BG28" s="19"/>
+      <c r="BH28" s="19"/>
+      <c r="BI28" s="19"/>
+      <c r="BJ28" s="19"/>
+      <c r="BK28" s="19"/>
+    </row>
+    <row r="29" spans="1:63" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>25</v>
       </c>
@@ -3310,8 +3785,22 @@
       <c r="AU29" s="19"/>
       <c r="AV29" s="19"/>
       <c r="AW29" s="19"/>
-    </row>
-    <row r="30" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="AX29" s="19"/>
+      <c r="AY29" s="19"/>
+      <c r="AZ29" s="19"/>
+      <c r="BA29" s="19"/>
+      <c r="BB29" s="19"/>
+      <c r="BC29" s="19"/>
+      <c r="BD29" s="19"/>
+      <c r="BE29" s="19"/>
+      <c r="BF29" s="19"/>
+      <c r="BG29" s="19"/>
+      <c r="BH29" s="19"/>
+      <c r="BI29" s="19"/>
+      <c r="BJ29" s="19"/>
+      <c r="BK29" s="19"/>
+    </row>
+    <row r="30" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>26</v>
       </c>
@@ -3373,14 +3862,28 @@
       <c r="AO30" s="19"/>
       <c r="AP30" s="19"/>
       <c r="AQ30" s="19"/>
-      <c r="AR30" s="40"/>
-      <c r="AS30" s="40"/>
+      <c r="AR30" s="31"/>
+      <c r="AS30" s="31"/>
       <c r="AT30" s="21"/>
       <c r="AU30" s="19"/>
       <c r="AV30" s="19"/>
       <c r="AW30" s="19"/>
-    </row>
-    <row r="31" spans="1:49" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="AX30" s="19"/>
+      <c r="AY30" s="19"/>
+      <c r="AZ30" s="19"/>
+      <c r="BA30" s="19"/>
+      <c r="BB30" s="19"/>
+      <c r="BC30" s="19"/>
+      <c r="BD30" s="19"/>
+      <c r="BE30" s="19"/>
+      <c r="BF30" s="19"/>
+      <c r="BG30" s="19"/>
+      <c r="BH30" s="19"/>
+      <c r="BI30" s="19"/>
+      <c r="BJ30" s="19"/>
+      <c r="BK30" s="19"/>
+    </row>
+    <row r="31" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>27</v>
       </c>
@@ -3391,7 +3894,7 @@
         <v>38</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>31</v>
@@ -3442,14 +3945,28 @@
       <c r="AO31" s="19"/>
       <c r="AP31" s="19"/>
       <c r="AQ31" s="19"/>
-      <c r="AR31" s="40"/>
-      <c r="AS31" s="40"/>
+      <c r="AR31" s="31"/>
+      <c r="AS31" s="31"/>
       <c r="AT31" s="19"/>
       <c r="AU31" s="19"/>
       <c r="AV31" s="19"/>
       <c r="AW31" s="19"/>
-    </row>
-    <row r="32" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AX31" s="19"/>
+      <c r="AY31" s="19"/>
+      <c r="AZ31" s="19"/>
+      <c r="BA31" s="19"/>
+      <c r="BB31" s="19"/>
+      <c r="BC31" s="19"/>
+      <c r="BD31" s="19"/>
+      <c r="BE31" s="19"/>
+      <c r="BF31" s="19"/>
+      <c r="BG31" s="19"/>
+      <c r="BH31" s="19"/>
+      <c r="BI31" s="19"/>
+      <c r="BJ31" s="19"/>
+      <c r="BK31" s="19"/>
+    </row>
+    <row r="32" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>28</v>
       </c>
@@ -3457,7 +3974,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>89</v>
@@ -3517,8 +4034,22 @@
       <c r="AU32" s="19"/>
       <c r="AV32" s="19"/>
       <c r="AW32" s="19"/>
-    </row>
-    <row r="33" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AX32" s="19"/>
+      <c r="AY32" s="19"/>
+      <c r="AZ32" s="19"/>
+      <c r="BA32" s="19"/>
+      <c r="BB32" s="19"/>
+      <c r="BC32" s="19"/>
+      <c r="BD32" s="19"/>
+      <c r="BE32" s="19"/>
+      <c r="BF32" s="19"/>
+      <c r="BG32" s="19"/>
+      <c r="BH32" s="19"/>
+      <c r="BI32" s="19"/>
+      <c r="BJ32" s="19"/>
+      <c r="BK32" s="19"/>
+    </row>
+    <row r="33" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>29</v>
       </c>
@@ -3526,7 +4057,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>90</v>
@@ -3586,8 +4117,22 @@
       <c r="AU33" s="19"/>
       <c r="AV33" s="19"/>
       <c r="AW33" s="19"/>
-    </row>
-    <row r="34" spans="1:49" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AX33" s="19"/>
+      <c r="AY33" s="19"/>
+      <c r="AZ33" s="19"/>
+      <c r="BA33" s="19"/>
+      <c r="BB33" s="19"/>
+      <c r="BC33" s="19"/>
+      <c r="BD33" s="19"/>
+      <c r="BE33" s="19"/>
+      <c r="BF33" s="19"/>
+      <c r="BG33" s="19"/>
+      <c r="BH33" s="19"/>
+      <c r="BI33" s="19"/>
+      <c r="BJ33" s="19"/>
+      <c r="BK33" s="19"/>
+    </row>
+    <row r="34" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>30</v>
       </c>
@@ -3595,7 +4140,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>91</v>
@@ -3607,10 +4152,10 @@
         <v>87</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>37</v>
@@ -3655,43 +4200,540 @@
       <c r="AU34" s="21"/>
       <c r="AV34" s="19"/>
       <c r="AW34" s="19"/>
-    </row>
-    <row r="35" spans="1:49" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J35" s="25"/>
-      <c r="K35" s="36" t="s">
+      <c r="AX34" s="19"/>
+      <c r="AY34" s="19"/>
+      <c r="AZ34" s="19"/>
+      <c r="BA34" s="19"/>
+      <c r="BB34" s="19"/>
+      <c r="BC34" s="19"/>
+      <c r="BD34" s="19"/>
+      <c r="BE34" s="19"/>
+      <c r="BF34" s="19"/>
+      <c r="BG34" s="19"/>
+      <c r="BH34" s="19"/>
+      <c r="BI34" s="19"/>
+      <c r="BJ34" s="19"/>
+      <c r="BK34" s="19"/>
+    </row>
+    <row r="35" spans="1:63" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>31</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="19"/>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="19"/>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="19"/>
+      <c r="AH35" s="19"/>
+      <c r="AI35" s="19"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
+      <c r="AL35" s="19"/>
+      <c r="AM35" s="19"/>
+      <c r="AN35" s="19"/>
+      <c r="AO35" s="19"/>
+      <c r="AP35" s="19"/>
+      <c r="AQ35" s="19"/>
+      <c r="AR35" s="19"/>
+      <c r="AS35" s="19"/>
+      <c r="AT35" s="19"/>
+      <c r="AU35" s="20"/>
+      <c r="AV35" s="19"/>
+      <c r="AW35" s="19"/>
+      <c r="AX35" s="19"/>
+      <c r="AY35" s="19"/>
+      <c r="AZ35" s="19"/>
+      <c r="BA35" s="19"/>
+      <c r="BB35" s="19"/>
+      <c r="BC35" s="19"/>
+      <c r="BD35" s="19"/>
+      <c r="BE35" s="19"/>
+      <c r="BF35" s="19"/>
+      <c r="BG35" s="19"/>
+      <c r="BH35" s="19"/>
+      <c r="BI35" s="19"/>
+      <c r="BJ35" s="19"/>
+      <c r="BK35" s="19"/>
+    </row>
+    <row r="36" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <v>32</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="19"/>
+      <c r="AA36" s="19"/>
+      <c r="AB36" s="19"/>
+      <c r="AC36" s="19"/>
+      <c r="AD36" s="19"/>
+      <c r="AE36" s="19"/>
+      <c r="AF36" s="19"/>
+      <c r="AG36" s="19"/>
+      <c r="AH36" s="19"/>
+      <c r="AI36" s="19"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
+      <c r="AL36" s="19"/>
+      <c r="AM36" s="19"/>
+      <c r="AN36" s="19"/>
+      <c r="AO36" s="19"/>
+      <c r="AP36" s="19"/>
+      <c r="AQ36" s="19"/>
+      <c r="AR36" s="19"/>
+      <c r="AS36" s="19"/>
+      <c r="AT36" s="19"/>
+      <c r="AU36" s="19"/>
+      <c r="AV36" s="20"/>
+      <c r="AW36" s="20"/>
+      <c r="AX36" s="21"/>
+      <c r="AY36" s="19"/>
+      <c r="AZ36" s="19"/>
+      <c r="BA36" s="19"/>
+      <c r="BB36" s="19"/>
+      <c r="BC36" s="19"/>
+      <c r="BD36" s="19"/>
+      <c r="BE36" s="19"/>
+      <c r="BF36" s="19"/>
+      <c r="BG36" s="19"/>
+      <c r="BH36" s="19"/>
+      <c r="BI36" s="19"/>
+      <c r="BJ36" s="19"/>
+      <c r="BK36" s="19"/>
+    </row>
+    <row r="37" spans="1:63" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>33</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AE37" s="19"/>
+      <c r="AF37" s="19"/>
+      <c r="AG37" s="19"/>
+      <c r="AH37" s="19"/>
+      <c r="AI37" s="19"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
+      <c r="AL37" s="19"/>
+      <c r="AM37" s="19"/>
+      <c r="AN37" s="19"/>
+      <c r="AO37" s="19"/>
+      <c r="AP37" s="19"/>
+      <c r="AQ37" s="19"/>
+      <c r="AR37" s="19"/>
+      <c r="AS37" s="19"/>
+      <c r="AT37" s="19"/>
+      <c r="AU37" s="19"/>
+      <c r="AV37" s="19"/>
+      <c r="AW37" s="19"/>
+      <c r="AX37" s="20"/>
+      <c r="AY37" s="20"/>
+      <c r="AZ37" s="19"/>
+      <c r="BA37" s="19"/>
+      <c r="BB37" s="19"/>
+      <c r="BC37" s="19"/>
+      <c r="BD37" s="19"/>
+      <c r="BE37" s="19"/>
+      <c r="BF37" s="19"/>
+      <c r="BG37" s="19"/>
+      <c r="BH37" s="19"/>
+      <c r="BI37" s="19"/>
+      <c r="BJ37" s="19"/>
+      <c r="BK37" s="19"/>
+    </row>
+    <row r="38" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>34</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AE38" s="19"/>
+      <c r="AF38" s="19"/>
+      <c r="AG38" s="19"/>
+      <c r="AH38" s="19"/>
+      <c r="AI38" s="19"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
+      <c r="AL38" s="19"/>
+      <c r="AM38" s="19"/>
+      <c r="AN38" s="19"/>
+      <c r="AO38" s="19"/>
+      <c r="AP38" s="19"/>
+      <c r="AQ38" s="19"/>
+      <c r="AR38" s="19"/>
+      <c r="AS38" s="19"/>
+      <c r="AT38" s="19"/>
+      <c r="AU38" s="19"/>
+      <c r="AV38" s="19"/>
+      <c r="AW38" s="19"/>
+      <c r="AX38" s="20"/>
+      <c r="AY38" s="20"/>
+      <c r="AZ38" s="19"/>
+      <c r="BA38" s="19"/>
+      <c r="BB38" s="19"/>
+      <c r="BC38" s="19"/>
+      <c r="BD38" s="19"/>
+      <c r="BE38" s="19"/>
+      <c r="BF38" s="19"/>
+      <c r="BG38" s="19"/>
+      <c r="BH38" s="19"/>
+      <c r="BI38" s="19"/>
+      <c r="BJ38" s="19"/>
+    </row>
+    <row r="39" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <v>35</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+      <c r="AD39" s="19"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="19"/>
+      <c r="AG39" s="19"/>
+      <c r="AH39" s="19"/>
+      <c r="AI39" s="19"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
+      <c r="AL39" s="19"/>
+      <c r="AM39" s="19"/>
+      <c r="AN39" s="19"/>
+      <c r="AO39" s="19"/>
+      <c r="AP39" s="19"/>
+      <c r="AQ39" s="19"/>
+      <c r="AR39" s="19"/>
+      <c r="AS39" s="19"/>
+      <c r="AT39" s="19"/>
+      <c r="AU39" s="19"/>
+      <c r="AV39" s="19"/>
+      <c r="AW39" s="19"/>
+      <c r="AX39" s="20"/>
+      <c r="AY39" s="20"/>
+      <c r="AZ39" s="19"/>
+      <c r="BA39" s="19"/>
+      <c r="BB39" s="19"/>
+      <c r="BC39" s="19"/>
+      <c r="BD39" s="19"/>
+      <c r="BE39" s="19"/>
+      <c r="BF39" s="19"/>
+      <c r="BG39" s="19"/>
+      <c r="BH39" s="19"/>
+      <c r="BI39" s="19"/>
+      <c r="BJ39" s="19"/>
+    </row>
+    <row r="40" spans="1:63" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>36</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
+      <c r="AA40" s="19"/>
+      <c r="AB40" s="19"/>
+      <c r="AC40" s="19"/>
+      <c r="AD40" s="19"/>
+      <c r="AE40" s="19"/>
+      <c r="AF40" s="19"/>
+      <c r="AG40" s="19"/>
+      <c r="AH40" s="19"/>
+      <c r="AI40" s="19"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
+      <c r="AL40" s="19"/>
+      <c r="AM40" s="19"/>
+      <c r="AN40" s="19"/>
+      <c r="AO40" s="19"/>
+      <c r="AP40" s="19"/>
+      <c r="AQ40" s="19"/>
+      <c r="AR40" s="19"/>
+      <c r="AS40" s="19"/>
+      <c r="AT40" s="19"/>
+      <c r="AU40" s="19"/>
+      <c r="AV40" s="19"/>
+      <c r="AW40" s="19"/>
+      <c r="AX40" s="20"/>
+      <c r="AY40" s="20"/>
+      <c r="AZ40" s="19"/>
+      <c r="BA40" s="19"/>
+      <c r="BB40" s="19"/>
+      <c r="BC40" s="19"/>
+      <c r="BD40" s="19"/>
+      <c r="BE40" s="19"/>
+      <c r="BF40" s="19"/>
+      <c r="BG40" s="19"/>
+      <c r="BH40" s="19"/>
+      <c r="BI40" s="19"/>
+      <c r="BJ40" s="19"/>
+    </row>
+    <row r="41" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J41" s="25"/>
+      <c r="K41" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-    </row>
-    <row r="36" spans="1:49" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J36" s="26"/>
-      <c r="K36" s="31" t="s">
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+    </row>
+    <row r="42" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="26"/>
+      <c r="K42" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-    </row>
-    <row r="37" spans="1:49" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J37" s="27"/>
-      <c r="K37" s="33" t="s">
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+    </row>
+    <row r="43" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="27"/>
+      <c r="K43" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="AQ2:BL2"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="U2:AP2"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="J2:T2"/>
+    <mergeCell ref="AQ2:BL2"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="U2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="J5">
     <cfRule type="dataBar" priority="1">
@@ -3751,26 +4793,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updating the PP according to latest deliveries Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85542FE1-416E-43D8-9DB3-83CF3EDCD5D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE1AD0-BEB0-44AA-AFEF-08C4F8190C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="117">
   <si>
     <t>#</t>
   </si>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>Completing the APIs section in the GDD</t>
-  </si>
-  <si>
-    <t>3-3-2020</t>
   </si>
   <si>
     <t>4-3-2020</t>
@@ -773,10 +770,10 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -785,10 +782,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1237,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:BL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,11 +1269,11 @@
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -1318,81 +1315,81 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="33">
+      <c r="J2" s="37">
         <v>43831</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33">
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37">
         <v>43862</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33">
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37">
         <v>43891</v>
       </c>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33"/>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
     </row>
     <row r="3" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11">
@@ -4004,7 +4001,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>89</v>
@@ -4433,7 +4430,9 @@
       <c r="G37" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H37" s="8"/>
+      <c r="H37" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="I37" s="8" t="s">
         <v>37</v>
       </c>
@@ -4479,9 +4478,9 @@
       <c r="AW37" s="19"/>
       <c r="AX37" s="20"/>
       <c r="AY37" s="20"/>
-      <c r="AZ37" s="19"/>
-      <c r="BA37" s="19"/>
-      <c r="BB37" s="19"/>
+      <c r="AZ37" s="20"/>
+      <c r="BA37" s="20"/>
+      <c r="BB37" s="21"/>
       <c r="BC37" s="19"/>
       <c r="BD37" s="19"/>
       <c r="BE37" s="19"/>
@@ -4512,9 +4511,11 @@
         <v>98</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H38" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="I38" s="8" t="s">
         <v>37</v>
       </c>
@@ -4560,8 +4561,8 @@
       <c r="AW38" s="19"/>
       <c r="AX38" s="20"/>
       <c r="AY38" s="20"/>
-      <c r="AZ38" s="19"/>
-      <c r="BA38" s="19"/>
+      <c r="AZ38" s="20"/>
+      <c r="BA38" s="20"/>
       <c r="BB38" s="19"/>
       <c r="BC38" s="19"/>
       <c r="BD38" s="19"/>
@@ -4580,10 +4581,10 @@
         <v>27</v>
       </c>
       <c r="C39" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>31</v>
@@ -4594,7 +4595,9 @@
       <c r="G39" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="I39" s="8"/>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
@@ -4638,8 +4641,8 @@
       <c r="AW39" s="19"/>
       <c r="AX39" s="20"/>
       <c r="AY39" s="20"/>
-      <c r="AZ39" s="19"/>
-      <c r="BA39" s="19"/>
+      <c r="AZ39" s="20"/>
+      <c r="BA39" s="20"/>
       <c r="BB39" s="19"/>
       <c r="BC39" s="19"/>
       <c r="BD39" s="19"/>
@@ -4650,7 +4653,7 @@
       <c r="BI39" s="19"/>
       <c r="BJ39" s="19"/>
     </row>
-    <row r="40" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>36</v>
       </c>
@@ -4658,10 +4661,10 @@
         <v>28</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>31</v>
@@ -4672,8 +4675,12 @@
       <c r="G40" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="H40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
@@ -4716,8 +4723,8 @@
       <c r="AW40" s="19"/>
       <c r="AX40" s="20"/>
       <c r="AY40" s="20"/>
-      <c r="AZ40" s="19"/>
-      <c r="BA40" s="19"/>
+      <c r="AZ40" s="20"/>
+      <c r="BA40" s="23"/>
       <c r="BB40" s="19"/>
       <c r="BC40" s="19"/>
       <c r="BD40" s="19"/>
@@ -4733,22 +4740,22 @@
         <v>37</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
@@ -4792,11 +4799,11 @@
       <c r="AU41" s="19"/>
       <c r="AV41" s="19"/>
       <c r="AW41" s="19"/>
-      <c r="AX41" s="19"/>
-      <c r="AY41" s="19"/>
-      <c r="AZ41" s="19"/>
-      <c r="BA41" s="19"/>
-      <c r="BB41" s="19"/>
+      <c r="AX41" s="20"/>
+      <c r="AY41" s="20"/>
+      <c r="AZ41" s="20"/>
+      <c r="BA41" s="20"/>
+      <c r="BB41" s="20"/>
       <c r="BC41" s="19"/>
       <c r="BD41" s="19"/>
       <c r="BE41" s="19"/>
@@ -4828,12 +4835,12 @@
     </row>
     <row r="46" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J46" s="27"/>
-      <c r="K46" s="36" t="s">
+      <c r="K46" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="L46" s="37"/>
-      <c r="M46" s="37"/>
-      <c r="N46" s="37"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5132,7 +5139,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>81</v>
@@ -5152,7 +5159,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Updating the PP after the latest review Creating GDD_Review sheet Creating CDD_Review sheet Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE1AD0-BEB0-44AA-AFEF-08C4F8190C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3826166C-7790-41E5-8F01-A12179229F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -349,12 +349,6 @@
     <t>GDD-Creation</t>
   </si>
   <si>
-    <t>CDD-DIO-Creation</t>
-  </si>
-  <si>
-    <t>Initiating the CDD document for the DIO driver</t>
-  </si>
-  <si>
     <t>Initiating the CDD document for the LCD driver</t>
   </si>
   <si>
@@ -383,6 +377,33 @@
   </si>
   <si>
     <t>15-3-2021</t>
+  </si>
+  <si>
+    <t>Initiating the CDD document for the Switch driver</t>
+  </si>
+  <si>
+    <t>CDD-Switch-Creation</t>
+  </si>
+  <si>
+    <t>CDD-LCD-Modifications</t>
+  </si>
+  <si>
+    <t>Considering the 1st point in the GDD_Review sheet</t>
+  </si>
+  <si>
+    <t>Considering the "APIs" points in the GDD_Review sheet</t>
+  </si>
+  <si>
+    <t>Considering the points in the CDD_Review sheet</t>
+  </si>
+  <si>
+    <t>6-3-2020</t>
+  </si>
+  <si>
+    <t>11-3-2020</t>
+  </si>
+  <si>
+    <t>9-3-2020</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:BL46"/>
+  <dimension ref="A1:BL49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4007,7 +4028,7 @@
         <v>89</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>81</v>
@@ -4090,7 +4111,7 @@
         <v>90</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>87</v>
@@ -4173,7 +4194,7 @@
         <v>91</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>87</v>
@@ -4256,7 +4277,7 @@
         <v>95</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>96</v>
@@ -4339,7 +4360,7 @@
         <v>97</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>96</v>
@@ -4422,7 +4443,7 @@
         <v>101</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>98</v>
@@ -4505,7 +4526,7 @@
         <v>102</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>98</v>
@@ -4581,13 +4602,13 @@
         <v>27</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>98</v>
@@ -4653,7 +4674,7 @@
       <c r="BI39" s="19"/>
       <c r="BJ39" s="19"/>
     </row>
-    <row r="40" spans="1:63" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>36</v>
       </c>
@@ -4661,13 +4682,13 @@
         <v>28</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>98</v>
@@ -4740,22 +4761,22 @@
         <v>37</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="F41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
@@ -4799,12 +4820,12 @@
       <c r="AU41" s="19"/>
       <c r="AV41" s="19"/>
       <c r="AW41" s="19"/>
-      <c r="AX41" s="20"/>
-      <c r="AY41" s="20"/>
-      <c r="AZ41" s="20"/>
-      <c r="BA41" s="20"/>
-      <c r="BB41" s="20"/>
-      <c r="BC41" s="19"/>
+      <c r="AX41" s="19"/>
+      <c r="AY41" s="19"/>
+      <c r="AZ41" s="19"/>
+      <c r="BA41" s="19"/>
+      <c r="BB41" s="19"/>
+      <c r="BC41" s="20"/>
       <c r="BD41" s="19"/>
       <c r="BE41" s="19"/>
       <c r="BF41" s="19"/>
@@ -4813,43 +4834,287 @@
       <c r="BI41" s="19"/>
       <c r="BJ41" s="19"/>
     </row>
-    <row r="42" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J44" s="25"/>
-      <c r="K44" s="38" t="s">
+    <row r="42" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
+        <v>38</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="19"/>
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="19"/>
+      <c r="AC42" s="19"/>
+      <c r="AD42" s="19"/>
+      <c r="AE42" s="19"/>
+      <c r="AF42" s="19"/>
+      <c r="AG42" s="19"/>
+      <c r="AH42" s="19"/>
+      <c r="AI42" s="19"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
+      <c r="AL42" s="19"/>
+      <c r="AM42" s="19"/>
+      <c r="AN42" s="19"/>
+      <c r="AO42" s="19"/>
+      <c r="AP42" s="19"/>
+      <c r="AQ42" s="19"/>
+      <c r="AR42" s="19"/>
+      <c r="AS42" s="19"/>
+      <c r="AT42" s="19"/>
+      <c r="AU42" s="19"/>
+      <c r="AV42" s="19"/>
+      <c r="AW42" s="19"/>
+      <c r="AX42" s="19"/>
+      <c r="AY42" s="19"/>
+      <c r="AZ42" s="19"/>
+      <c r="BA42" s="19"/>
+      <c r="BB42" s="19"/>
+      <c r="BC42" s="20"/>
+      <c r="BD42" s="19"/>
+      <c r="BE42" s="19"/>
+      <c r="BF42" s="19"/>
+      <c r="BG42" s="19"/>
+      <c r="BH42" s="19"/>
+      <c r="BI42" s="19"/>
+      <c r="BJ42" s="19"/>
+    </row>
+    <row r="43" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <v>39</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="19"/>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="19"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AM43" s="19"/>
+      <c r="AN43" s="19"/>
+      <c r="AO43" s="19"/>
+      <c r="AP43" s="19"/>
+      <c r="AQ43" s="19"/>
+      <c r="AR43" s="19"/>
+      <c r="AS43" s="19"/>
+      <c r="AT43" s="19"/>
+      <c r="AU43" s="19"/>
+      <c r="AV43" s="19"/>
+      <c r="AW43" s="19"/>
+      <c r="AX43" s="19"/>
+      <c r="AY43" s="19"/>
+      <c r="AZ43" s="19"/>
+      <c r="BA43" s="19"/>
+      <c r="BB43" s="19"/>
+      <c r="BC43" s="20"/>
+      <c r="BD43" s="19"/>
+      <c r="BE43" s="19"/>
+      <c r="BF43" s="19"/>
+      <c r="BG43" s="19"/>
+      <c r="BH43" s="19"/>
+      <c r="BI43" s="19"/>
+      <c r="BJ43" s="19"/>
+    </row>
+    <row r="44" spans="1:63" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="18">
+        <v>40</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="19"/>
+      <c r="AC44" s="19"/>
+      <c r="AD44" s="19"/>
+      <c r="AE44" s="19"/>
+      <c r="AF44" s="19"/>
+      <c r="AG44" s="19"/>
+      <c r="AH44" s="19"/>
+      <c r="AI44" s="19"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
+      <c r="AL44" s="19"/>
+      <c r="AM44" s="19"/>
+      <c r="AN44" s="19"/>
+      <c r="AO44" s="19"/>
+      <c r="AP44" s="19"/>
+      <c r="AQ44" s="19"/>
+      <c r="AR44" s="19"/>
+      <c r="AS44" s="19"/>
+      <c r="AT44" s="19"/>
+      <c r="AU44" s="19"/>
+      <c r="AV44" s="19"/>
+      <c r="AW44" s="19"/>
+      <c r="AX44" s="19"/>
+      <c r="AY44" s="19"/>
+      <c r="AZ44" s="19"/>
+      <c r="BA44" s="19"/>
+      <c r="BB44" s="19"/>
+      <c r="BC44" s="20"/>
+      <c r="BD44" s="19"/>
+      <c r="BE44" s="19"/>
+      <c r="BF44" s="19"/>
+      <c r="BG44" s="19"/>
+      <c r="BH44" s="19"/>
+      <c r="BI44" s="19"/>
+      <c r="BJ44" s="19"/>
+    </row>
+    <row r="45" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="25"/>
+      <c r="K47" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-    </row>
-    <row r="45" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J45" s="26"/>
-      <c r="K45" s="34" t="s">
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+    </row>
+    <row r="48" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="26"/>
+      <c r="K48" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-    </row>
-    <row r="46" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J46" s="27"/>
-      <c r="K46" s="32" t="s">
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+    </row>
+    <row r="49" spans="10:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="27"/>
+      <c r="K49" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K48:N48"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="J2:T2"/>
     <mergeCell ref="AQ2:BL2"/>
-    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="U2:AP2"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -5139,7 +5404,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>81</v>
@@ -5159,7 +5424,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Updating the RTM and PP after the latest deliveries Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP/PP.xlsx
+++ b/Software Deliveries Log/PP/PP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\PP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3826166C-7790-41E5-8F01-A12179229F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45372629-565B-4E7C-A695-D09D3471A556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -400,10 +400,10 @@
     <t>6-3-2020</t>
   </si>
   <si>
-    <t>11-3-2020</t>
-  </si>
-  <si>
     <t>9-3-2020</t>
+  </si>
+  <si>
+    <t>8-3-2020</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:BL49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="F34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BE43" sqref="BE41:BE43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4826,8 +4826,8 @@
       <c r="BA41" s="19"/>
       <c r="BB41" s="19"/>
       <c r="BC41" s="20"/>
-      <c r="BD41" s="19"/>
-      <c r="BE41" s="19"/>
+      <c r="BD41" s="20"/>
+      <c r="BE41" s="20"/>
       <c r="BF41" s="19"/>
       <c r="BG41" s="19"/>
       <c r="BH41" s="19"/>
@@ -4854,7 +4854,7 @@
         <v>121</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="8" t="s">
@@ -4906,8 +4906,8 @@
       <c r="BA42" s="19"/>
       <c r="BB42" s="19"/>
       <c r="BC42" s="20"/>
-      <c r="BD42" s="19"/>
-      <c r="BE42" s="19"/>
+      <c r="BD42" s="20"/>
+      <c r="BE42" s="20"/>
       <c r="BF42" s="19"/>
       <c r="BG42" s="19"/>
       <c r="BH42" s="19"/>
@@ -4934,7 +4934,7 @@
         <v>66</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H43" s="8"/>
       <c r="I43" s="8" t="s">
@@ -4986,8 +4986,8 @@
       <c r="BA43" s="19"/>
       <c r="BB43" s="19"/>
       <c r="BC43" s="20"/>
-      <c r="BD43" s="19"/>
-      <c r="BE43" s="19"/>
+      <c r="BD43" s="20"/>
+      <c r="BE43" s="20"/>
       <c r="BF43" s="19"/>
       <c r="BG43" s="19"/>
       <c r="BH43" s="19"/>
@@ -5014,7 +5014,7 @@
         <v>121</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8" t="s">
@@ -5066,7 +5066,7 @@
       <c r="BA44" s="19"/>
       <c r="BB44" s="19"/>
       <c r="BC44" s="20"/>
-      <c r="BD44" s="19"/>
+      <c r="BD44" s="20"/>
       <c r="BE44" s="19"/>
       <c r="BF44" s="19"/>
       <c r="BG44" s="19"/>

</xml_diff>